<commit_message>
docs: grammar topics finalized
</commit_message>
<xml_diff>
--- a/src/components/01_config/TwoThousands.xlsx
+++ b/src/components/01_config/TwoThousands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\src\components\01_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4CD5C2-5342-4608-9D40-7E38EDEE4F30}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34CE7C9-1A90-4A02-974C-B184D69CE6C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="3" xr2:uid="{3025596F-8F86-4685-8931-8FCF7E89A1B1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12288" windowHeight="5904" activeTab="3" xr2:uid="{3025596F-8F86-4685-8931-8FCF7E89A1B1}"/>
   </bookViews>
   <sheets>
     <sheet name=" Слова" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4773" uniqueCount="4757">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4781" uniqueCount="4770">
   <si>
     <t>з</t>
   </si>
@@ -14223,21 +14223,6 @@
     <t>Present simple</t>
   </si>
   <si>
-    <t>Present past</t>
-  </si>
-  <si>
-    <t>Present future</t>
-  </si>
-  <si>
-    <t>Future Continues</t>
-  </si>
-  <si>
-    <t>Present continues</t>
-  </si>
-  <si>
-    <t>Past Continues</t>
-  </si>
-  <si>
     <t>Present Perfect</t>
   </si>
   <si>
@@ -14262,15 +14247,6 @@
     <t>Singular and Plural nouns</t>
   </si>
   <si>
-    <t>Negative and interrogative sentences</t>
-  </si>
-  <si>
-    <t>Present Tense</t>
-  </si>
-  <si>
-    <t>Continues Tense</t>
-  </si>
-  <si>
     <t>All Tenses</t>
   </si>
   <si>
@@ -14280,9 +14256,6 @@
     <t>Active Voice and Passive Voice</t>
   </si>
   <si>
-    <t>Have got</t>
-  </si>
-  <si>
     <t>Modal verbs</t>
   </si>
   <si>
@@ -14292,13 +14265,79 @@
     <t>Imperative sentences</t>
   </si>
   <si>
-    <t>8 basic rules (part 1)</t>
-  </si>
-  <si>
-    <t>8 basic rules (part 2)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> `https://www.busuu.com/en/english/grammar-rules</t>
+  </si>
+  <si>
+    <t>Repeat: Continues Tense</t>
+  </si>
+  <si>
+    <t>Repeat: Simple Tense</t>
+  </si>
+  <si>
+    <t>Repeat: Irregular verbs</t>
+  </si>
+  <si>
+    <t>Repeat: date and time</t>
+  </si>
+  <si>
+    <t>Repeat: modal verbs</t>
+  </si>
+  <si>
+    <t>Repeat: Singular &amp; Plural, Comperative &amp; Superlative</t>
+  </si>
+  <si>
+    <t>Repeat: Prepositions of Place</t>
+  </si>
+  <si>
+    <t>Repeat: Active and passive voice</t>
+  </si>
+  <si>
+    <t>Repeat: Present Perfect</t>
+  </si>
+  <si>
+    <t>8 basic rules of Grammar (part 1)</t>
+  </si>
+  <si>
+    <t>8 basic rules of Grammar (part 2)</t>
+  </si>
+  <si>
+    <t>To be</t>
+  </si>
+  <si>
+    <t>Future Perfect and Past Perfect</t>
+  </si>
+  <si>
+    <t>Future simple</t>
+  </si>
+  <si>
+    <t>Past simple</t>
+  </si>
+  <si>
+    <t>Simple Tense</t>
+  </si>
+  <si>
+    <t>Negative and interrogative sentences - Simple</t>
+  </si>
+  <si>
+    <t>Negative and interrogative sentences - Continuous</t>
+  </si>
+  <si>
+    <t>Continuous Tense</t>
+  </si>
+  <si>
+    <t>Past Continuous</t>
+  </si>
+  <si>
+    <t>Future Continuous</t>
+  </si>
+  <si>
+    <t>Present Continuous</t>
+  </si>
+  <si>
+    <t>Negative and interrogative sentences - All Tenses</t>
+  </si>
+  <si>
+    <t>Repeat: Negative and interrogative sentences - All Tenses</t>
   </si>
 </sst>
 </file>
@@ -42542,15 +42581,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2065B795-6495-421C-8C31-54BC300F0CEC}">
-  <dimension ref="A2:C52"/>
+  <dimension ref="A2:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="39.109375" customWidth="1"/>
+    <col min="2" max="2" width="49.6640625" customWidth="1"/>
+    <col min="3" max="3" width="46.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -42571,7 +42611,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4730</v>
+        <v>4757</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -42579,7 +42619,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>4732</v>
+        <v>4730</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -42587,7 +42627,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>4731</v>
+        <v>4759</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -42595,7 +42635,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>4745</v>
+        <v>4760</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -42603,7 +42643,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>4745</v>
+        <v>4732</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -42611,7 +42651,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>4744</v>
+        <v>4761</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -42619,7 +42659,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>4744</v>
+        <v>4762</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -42627,7 +42667,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>4734</v>
+        <v>4767</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -42635,7 +42675,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>4733</v>
+        <v>4766</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -42643,7 +42683,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>4735</v>
+        <v>4765</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -42651,7 +42691,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>4746</v>
+        <v>4764</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -42659,7 +42699,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>4746</v>
+        <v>4763</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -42667,244 +42707,218 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>4736</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4731</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>4736</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4739</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>4747</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4768</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>4747</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4733</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>4737</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4734</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>4738</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4735</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>4739</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4736</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>4740</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4737</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>4741</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4738</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
-        <v>4742</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="7" t="s">
+        <v>4740</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
-        <v>4743</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="7" t="s">
+        <v>4741</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>4748</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4742</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>4749</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4743</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>4750</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4744</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>4751</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4755</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4745</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>4752</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4756</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" t="s">
         <v>4753</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>4754</v>
-      </c>
-      <c r="C33" t="s">
-        <v>4756</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>4752</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>4755</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>4751</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>4750</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>4749</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>4748</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>4747</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>4746</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>4754</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>4769</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <v>50</v>
+      <c r="B42" t="s">
+        <v>4758</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs: grammar topics reformatted
</commit_message>
<xml_diff>
--- a/src/components/01_config/TwoThousands.xlsx
+++ b/src/components/01_config/TwoThousands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\src\components\01_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34CE7C9-1A90-4A02-974C-B184D69CE6C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD14D71A-D3E5-4613-B125-23476C5CBC08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12288" windowHeight="5904" activeTab="3" xr2:uid="{3025596F-8F86-4685-8931-8FCF7E89A1B1}"/>
   </bookViews>
@@ -42581,10 +42581,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2065B795-6495-421C-8C31-54BC300F0CEC}">
-  <dimension ref="A2:C42"/>
+  <dimension ref="A2:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42593,332 +42593,492 @@
     <col min="3" max="3" width="46.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>4728</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>4729</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="str">
+        <f>"    - "&amp;B3</f>
+        <v xml:space="preserve">    - Pronouns</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>4757</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" t="str">
+        <f t="shared" ref="C4:C42" si="0">"    - "&amp;B4</f>
+        <v xml:space="preserve">    - To be</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>4730</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Present simple</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>4759</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Future simple</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>4760</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Past simple</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>4732</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Irregular verbs</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>4761</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Simple Tense</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>4762</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Negative and interrogative sentences - Simple</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>4767</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Present Continuous</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>4766</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Future Continuous</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>4765</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Past Continuous</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>4764</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Continuous Tense</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>4763</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Negative and interrogative sentences - Continuous</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>4731</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Present Perfect</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>4739</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - All Tenses</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>4768</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Negative and interrogative sentences - All Tenses</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>4733</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Prepositions of place</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>4734</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - What is the time</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>4735</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Dates in English</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>4736</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - There is/there are</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>4737</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Articles</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>4738</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Singular and Plural nouns</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>4740</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Comparative and Superlative Adjectives</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>4741</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Active Voice and Passive Voice</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>4742</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Modal verbs</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>4743</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Would and Used to</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>4744</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Imperative sentences</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>4755</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - 8 basic rules of Grammar (part 1)</v>
+      </c>
+      <c r="D30" t="s">
         <v>4745</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>4756</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - 8 basic rules of Grammar (part 2)</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>4753</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Repeat: Active and passive voice</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33" t="s">
         <v>4752</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Repeat: Prepositions of Place</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>4751</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Repeat: Singular &amp; Plural, Comperative &amp; Superlative</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>4750</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Repeat: modal verbs</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>4749</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Repeat: date and time</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" t="s">
         <v>4748</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Repeat: Irregular verbs</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" t="s">
         <v>4747</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Repeat: Simple Tense</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" t="s">
         <v>4746</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Repeat: Continues Tense</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" t="s">
         <v>4754</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Repeat: Present Perfect</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41" t="s">
         <v>4769</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Repeat: Negative and interrogative sentences - All Tenses</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42" t="s">
         <v>4758</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    - Future Perfect and Past Perfect</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(myprog): CurrentLesson button created
</commit_message>
<xml_diff>
--- a/src/components/01_config/TwoThousands.xlsx
+++ b/src/components/01_config/TwoThousands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\src\components\01_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD14D71A-D3E5-4613-B125-23476C5CBC08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DFA7D7-2B78-4950-AD85-85FE4CEF8DA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12288" windowHeight="5904" activeTab="3" xr2:uid="{3025596F-8F86-4685-8931-8FCF7E89A1B1}"/>
   </bookViews>
@@ -41631,8 +41631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC2A7625-49C4-422F-A6BE-B78D36DAC3F6}">
   <dimension ref="D2:E134"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
feat(myprogress): roadmap steps continued
</commit_message>
<xml_diff>
--- a/src/components/01_config/TwoThousands.xlsx
+++ b/src/components/01_config/TwoThousands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\src\components\01_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DFA7D7-2B78-4950-AD85-85FE4CEF8DA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D496818-AA8F-4490-BFBC-41ECFE037E35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12288" windowHeight="5904" activeTab="3" xr2:uid="{3025596F-8F86-4685-8931-8FCF7E89A1B1}"/>
   </bookViews>
@@ -14214,9 +14214,6 @@
     <t>хто</t>
   </si>
   <si>
-    <t>50 TOPICS</t>
-  </si>
-  <si>
     <t>Pronouns</t>
   </si>
   <si>
@@ -14338,6 +14335,9 @@
   </si>
   <si>
     <t>Repeat: Negative and interrogative sentences - All Tenses</t>
+  </si>
+  <si>
+    <t>40 LESSONS</t>
   </si>
 </sst>
 </file>
@@ -42584,7 +42584,7 @@
   <dimension ref="A2:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A2" sqref="A2:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42595,7 +42595,7 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
-        <v>4728</v>
+        <v>4769</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -42603,7 +42603,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4729</v>
+        <v>4728</v>
       </c>
       <c r="C3" t="str">
         <f>"    - "&amp;B3</f>
@@ -42615,7 +42615,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4757</v>
+        <v>4756</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ref="C4:C42" si="0">"    - "&amp;B4</f>
@@ -42627,7 +42627,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>4730</v>
+        <v>4729</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -42639,7 +42639,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>4759</v>
+        <v>4758</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -42651,7 +42651,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>4760</v>
+        <v>4759</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -42663,7 +42663,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>4732</v>
+        <v>4731</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -42675,7 +42675,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>4761</v>
+        <v>4760</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -42687,7 +42687,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>4762</v>
+        <v>4761</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -42699,7 +42699,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>4767</v>
+        <v>4766</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -42711,7 +42711,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>4766</v>
+        <v>4765</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -42723,7 +42723,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>4765</v>
+        <v>4764</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -42735,7 +42735,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>4764</v>
+        <v>4763</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -42747,7 +42747,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>4763</v>
+        <v>4762</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
@@ -42759,7 +42759,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>4731</v>
+        <v>4730</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -42771,7 +42771,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>4739</v>
+        <v>4738</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -42783,7 +42783,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>4768</v>
+        <v>4767</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -42795,7 +42795,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>4733</v>
+        <v>4732</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -42807,7 +42807,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>4734</v>
+        <v>4733</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
@@ -42819,7 +42819,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>4735</v>
+        <v>4734</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -42831,7 +42831,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>4736</v>
+        <v>4735</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
@@ -42843,7 +42843,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>4737</v>
+        <v>4736</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
@@ -42855,7 +42855,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>4738</v>
+        <v>4737</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
@@ -42867,7 +42867,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>4740</v>
+        <v>4739</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
@@ -42879,7 +42879,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>4741</v>
+        <v>4740</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
@@ -42891,7 +42891,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>4742</v>
+        <v>4741</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
@@ -42903,7 +42903,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
@@ -42915,7 +42915,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>4744</v>
+        <v>4743</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
@@ -42927,14 +42927,14 @@
         <v>28</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>4755</v>
+        <v>4754</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - 8 basic rules of Grammar (part 1)</v>
       </c>
       <c r="D30" t="s">
-        <v>4745</v>
+        <v>4744</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -42942,7 +42942,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>4756</v>
+        <v>4755</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
@@ -42954,7 +42954,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>4753</v>
+        <v>4752</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
@@ -42966,7 +42966,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>4752</v>
+        <v>4751</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
@@ -42978,7 +42978,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>4751</v>
+        <v>4750</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
@@ -42990,7 +42990,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>4750</v>
+        <v>4749</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
@@ -43002,7 +43002,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>4749</v>
+        <v>4748</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
@@ -43014,7 +43014,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>4748</v>
+        <v>4747</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="0"/>
@@ -43026,7 +43026,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>4747</v>
+        <v>4746</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="0"/>
@@ -43038,7 +43038,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>4746</v>
+        <v>4745</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="0"/>
@@ -43050,7 +43050,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>4754</v>
+        <v>4753</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="0"/>
@@ -43062,7 +43062,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>4769</v>
+        <v>4768</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="0"/>
@@ -43074,7 +43074,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>4758</v>
+        <v>4757</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="0"/>

</xml_diff>